<commit_message>
cbd build refactor done
</commit_message>
<xml_diff>
--- a/pur_doc/data/04_constant.xlsx
+++ b/pur_doc/data/04_constant.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B596AC-EFDE-412E-B8E4-4374225C7D2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E60887-FB92-4C25-A953-EE9CEF2DE2E4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hella_person" sheetId="4" r:id="rId1"/>
-    <sheet name="mgs" sheetId="3" r:id="rId2"/>
-    <sheet name="plant" sheetId="1" r:id="rId3"/>
-    <sheet name="ex_rate" sheetId="2" r:id="rId4"/>
+    <sheet name="mgs_sqe" sheetId="3" r:id="rId2"/>
+    <sheet name="mgm" sheetId="5" r:id="rId3"/>
+    <sheet name="plant" sheetId="1" r:id="rId4"/>
+    <sheet name="ex_rate" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">hella_person!$A$1:$D$40</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">mgs!$A$1:$E$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">mgs_sqe!$B$1:$D$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="267">
   <si>
     <t>plant</t>
   </si>
@@ -46,9 +47,6 @@
     <t>HSE</t>
   </si>
   <si>
-    <t>Hella Shanghai Electronics Co., Ltd.</t>
-  </si>
-  <si>
     <t>CNY</t>
   </si>
   <si>
@@ -79,15 +77,6 @@
     <t>HAE</t>
   </si>
   <si>
-    <t>HED</t>
-  </si>
-  <si>
-    <t>Hxx Axx Exx</t>
-  </si>
-  <si>
-    <t>Hxx Exx Dxx</t>
-  </si>
-  <si>
     <t>LASER</t>
   </si>
   <si>
@@ -725,6 +714,126 @@
   </si>
   <si>
     <t>Scott Zhao</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1029</t>
+  </si>
+  <si>
+    <t>1272</t>
+  </si>
+  <si>
+    <t>1132</t>
+  </si>
+  <si>
+    <t>1303</t>
+  </si>
+  <si>
+    <t>1253</t>
+  </si>
+  <si>
+    <t>1452</t>
+  </si>
+  <si>
+    <t>1463</t>
+  </si>
+  <si>
+    <t>1354</t>
+  </si>
+  <si>
+    <t>1193</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>1251</t>
+  </si>
+  <si>
+    <t>1361</t>
+  </si>
+  <si>
+    <t>1123</t>
+  </si>
+  <si>
+    <t>HELLA GmbH &amp; Co. KGaA</t>
+  </si>
+  <si>
+    <t>HKG</t>
+  </si>
+  <si>
+    <t>Hella Fahrzeugkomp. GmbH</t>
+  </si>
+  <si>
+    <t>HFK</t>
+  </si>
+  <si>
+    <t>Hella Aglaia Mob.Vis.GmbH</t>
+  </si>
+  <si>
+    <t>HAGL</t>
+  </si>
+  <si>
+    <t>Hella Automotive Mexico</t>
+  </si>
+  <si>
+    <t>HAM</t>
+  </si>
+  <si>
+    <t>Hella Electronics Mexico</t>
+  </si>
+  <si>
+    <t>HEM / merged to 1132</t>
+  </si>
+  <si>
+    <t>HELLA Romania SRL</t>
+  </si>
+  <si>
+    <t>HRO</t>
+  </si>
+  <si>
+    <t>UAB HELLA Lithuania</t>
+  </si>
+  <si>
+    <t>HLT</t>
+  </si>
+  <si>
+    <t>Hella BHAP(Jiangsu)Elect.</t>
+  </si>
+  <si>
+    <t>(Jiangsu) HBECN</t>
+  </si>
+  <si>
+    <t>Hella do Brazil Automotiv</t>
+  </si>
+  <si>
+    <t>HBRA</t>
+  </si>
+  <si>
+    <t>Hella India Autom. PrLtd</t>
+  </si>
+  <si>
+    <t>HIA</t>
+  </si>
+  <si>
+    <t>Hella Shanghai Electr.Co.</t>
+  </si>
+  <si>
+    <t>Hella (Xiamen) Atm.El. Lt</t>
+  </si>
+  <si>
+    <t>Hella (Xiamen)Electr.Dev.</t>
+  </si>
+  <si>
+    <t>HEDCN</t>
+  </si>
+  <si>
+    <t>Hella Electronics Corp.</t>
+  </si>
+  <si>
+    <t>HEC</t>
   </si>
 </sst>
 </file>
@@ -783,137 +892,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1492,7 +1471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3625C09-7D5A-4AEA-B557-20785648F30A}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -1507,587 +1486,587 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" t="s">
         <v>142</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" t="s">
         <v>142</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D10" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B12" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" t="s">
         <v>143</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D13" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D14" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D16" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D17" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D18" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D19" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D20" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D21" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D22" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D24" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C26" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D26" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C27" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D29" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D30" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D31" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D34" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C35" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D35" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D36" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B37" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B38" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D38" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B39" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B40" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D40" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B23:D23 D22 D24 B20:D21 B25:D25 B26 D26:D27 B1:D17 B18 D18 B27:D34 B36:D1048576">
-    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35 D35">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2101,890 +2080,1167 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F1C00D-2727-428E-BE4C-36B842D38574}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1111</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1111</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1111</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1111</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1111</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1111</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1111</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1111</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1111</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1111</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1111</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1111</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1111</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1111</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1111</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1111</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1111</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1111</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1111</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1111</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1111</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1111</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1111</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1111</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1111</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1111</v>
+      </c>
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1111</v>
+      </c>
+      <c r="B36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1111</v>
+      </c>
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1111</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1111</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1111</v>
+      </c>
+      <c r="B40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:D40" xr:uid="{46A10708-8CAD-4083-82D0-C1072359759A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D40">
+      <sortCondition ref="B1:B40"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="C1:D9 D10 D13:D14 C15:D34 C36:D1048576 C11:D12">
+    <cfRule type="cellIs" dxfId="24" priority="42" operator="equal">
+      <formula>"PlzUpdate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="23" priority="37" operator="equal">
+      <formula>"PlzUpdate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="cellIs" dxfId="22" priority="36" operator="equal">
+      <formula>"PlzUpdate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+      <formula>"PlzUpdate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:D35">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+      <formula>"PlzUpdate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Arial"&amp;9&amp;K737373 Copyright Protection: Confidential - ISO 16016&amp;1#</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD78265-D7BB-4972-895F-0FD9CFE2065C}">
+  <dimension ref="A1:C40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" t="s">
         <v>126</v>
       </c>
-      <c r="C2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" t="s">
         <v>126</v>
       </c>
-      <c r="C3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" t="s">
         <v>126</v>
       </c>
-      <c r="C4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="B39" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="B40" t="s">
         <v>122</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>126</v>
-      </c>
-      <c r="C14" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" t="s">
-        <v>140</v>
-      </c>
-      <c r="E15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" t="s">
-        <v>134</v>
-      </c>
-      <c r="D16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C17" t="s">
-        <v>139</v>
-      </c>
-      <c r="D17" t="s">
-        <v>140</v>
-      </c>
-      <c r="E17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18" t="s">
-        <v>139</v>
-      </c>
-      <c r="D18" t="s">
-        <v>140</v>
-      </c>
-      <c r="E18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" t="s">
-        <v>140</v>
-      </c>
-      <c r="E19" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" t="s">
-        <v>139</v>
-      </c>
-      <c r="D20" t="s">
-        <v>140</v>
-      </c>
-      <c r="E20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" t="s">
-        <v>133</v>
-      </c>
-      <c r="E21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>126</v>
-      </c>
-      <c r="C22" t="s">
-        <v>127</v>
-      </c>
-      <c r="D22" t="s">
-        <v>130</v>
-      </c>
-      <c r="E22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23" t="s">
-        <v>127</v>
-      </c>
-      <c r="D23" t="s">
-        <v>130</v>
-      </c>
-      <c r="E23" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" t="s">
-        <v>133</v>
-      </c>
-      <c r="E24" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" t="s">
-        <v>124</v>
-      </c>
-      <c r="E26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" t="s">
-        <v>126</v>
-      </c>
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" t="s">
-        <v>124</v>
-      </c>
-      <c r="E27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" t="s">
-        <v>126</v>
-      </c>
-      <c r="C28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" t="s">
-        <v>124</v>
-      </c>
-      <c r="E28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>117</v>
-      </c>
-      <c r="C29" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" t="s">
-        <v>111</v>
-      </c>
-      <c r="E29" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>126</v>
-      </c>
-      <c r="C30" t="s">
-        <v>134</v>
-      </c>
-      <c r="D30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E30" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" t="s">
-        <v>127</v>
-      </c>
-      <c r="D31" t="s">
-        <v>130</v>
-      </c>
-      <c r="E31" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" t="s">
-        <v>126</v>
-      </c>
-      <c r="C32" t="s">
-        <v>127</v>
-      </c>
-      <c r="D32" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" t="s">
-        <v>126</v>
-      </c>
-      <c r="C33" t="s">
-        <v>127</v>
-      </c>
-      <c r="D33" t="s">
-        <v>130</v>
-      </c>
-      <c r="E33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" t="s">
-        <v>126</v>
-      </c>
-      <c r="C34" t="s">
-        <v>127</v>
-      </c>
-      <c r="D34" t="s">
-        <v>130</v>
-      </c>
-      <c r="E34" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" t="s">
-        <v>117</v>
-      </c>
-      <c r="C35" t="s">
-        <v>121</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E35" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36" t="s">
-        <v>126</v>
-      </c>
-      <c r="C36" t="s">
-        <v>139</v>
-      </c>
-      <c r="D36" t="s">
-        <v>141</v>
-      </c>
-      <c r="E36" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" t="s">
-        <v>117</v>
-      </c>
-      <c r="C37" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" t="s">
-        <v>113</v>
-      </c>
-      <c r="E37" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38" t="s">
-        <v>124</v>
-      </c>
-      <c r="E38" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>24</v>
-      </c>
-      <c r="B39" t="s">
-        <v>126</v>
-      </c>
-      <c r="C39" t="s">
-        <v>139</v>
-      </c>
-      <c r="D39" t="s">
-        <v>141</v>
-      </c>
-      <c r="E39" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" t="s">
-        <v>126</v>
       </c>
       <c r="C40" t="s">
         <v>134</v>
       </c>
-      <c r="D40" t="s">
-        <v>138</v>
-      </c>
-      <c r="E40" t="s">
-        <v>137</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E40" xr:uid="{46A10708-8CAD-4083-82D0-C1072359759A}">
-    <sortState ref="A2:E40">
-      <sortCondition ref="A1:A40"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="C7:E8 C5 E5 E10 C25:E26 C36:E1048576 E13:E14 C1:E4 C11:E12 C20:E22 C29:E29">
-    <cfRule type="cellIs" dxfId="37" priority="42" operator="equal">
+  <conditionalFormatting sqref="C36:C1048576 C1:C4 C11:C12 C14:C34 C6:C9">
+    <cfRule type="cellIs" dxfId="19" priority="38" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B5 B7:B8 B25:B26 B36:B39 B29 B20:B22 B10:B12">
-    <cfRule type="cellIs" dxfId="36" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="37" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="36" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23:E23">
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="32" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="cellIs" dxfId="29" priority="32" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31:E31 C33:E33">
-    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="30" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31 B33">
-    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32:E32 C34:E34">
-    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="28" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32 B34">
-    <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24:E24">
-    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="26" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14:D14">
-    <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="24" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="22" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:E30">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="21" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16:E16">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27:E27">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28:E28">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18:E18">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19:E19">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17:E17">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:E15">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:E9">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"PlzUpdate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35 E35">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"PlzUpdate"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3001,19 +3257,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3028,36 +3284,157 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1111</v>
+      <c r="A2" t="s">
+        <v>227</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>241</v>
       </c>
       <c r="C2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B10" t="s">
+        <v>257</v>
+      </c>
+      <c r="C10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B12" t="s">
+        <v>261</v>
+      </c>
+      <c r="C12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1251</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1361</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C14" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B15" t="s">
+        <v>265</v>
+      </c>
+      <c r="C15" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3069,12 +3446,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F508815-5082-4788-8582-AD235A125B68}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3086,15 +3463,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>8.14</v>
@@ -3102,7 +3479,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>1.18</v>
@@ -3110,7 +3487,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3118,7 +3495,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>128</v>
@@ -3126,7 +3503,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>0.9</v>
@@ -3134,7 +3511,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>1.57</v>
@@ -3142,7 +3519,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>1.61</v>

</xml_diff>